<commit_message>
data de rips modificada
</commit_message>
<xml_diff>
--- a/cruz_verde_prueba.xlsx
+++ b/cruz_verde_prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GREGORY\Desktop\prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2162AD-E9BE-41DC-ABEC-2A11735C0DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F077FC-94C5-4437-A984-A4EA9E5DDD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="2640" windowWidth="28695" windowHeight="13560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="1170" windowWidth="28695" windowHeight="13560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11105" uniqueCount="1418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11051" uniqueCount="1418">
   <si>
     <t>Plan</t>
   </si>
@@ -4779,7 +4779,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4787,6 +4787,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -51880,10 +51882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F44231-3A66-4658-9AD4-A8252BD13989}">
-  <dimension ref="A1:BE8"/>
+  <dimension ref="A1:BE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52067,467 +52069,467 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>1029409136</v>
-      </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2">
+      <c r="F2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="5">
+        <v>30020376</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="I2" s="5">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="1">
-        <v>43754</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="J2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="7">
+        <v>17891</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2">
-        <v>5507</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>1415</v>
+      </c>
+      <c r="R2" s="5">
+        <v>4862</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="2">
-        <v>44712.42292824074</v>
-      </c>
-      <c r="V2" s="4">
-        <v>7703038010302</v>
-      </c>
-      <c r="W2" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2">
-        <v>5</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD2">
+      <c r="T2" s="8">
+        <v>44697.391111111108</v>
+      </c>
+      <c r="V2" s="6">
+        <v>7702605184965</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>20</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT2" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="BC2" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5">
+        <v>30020376</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="I3" s="5">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="7">
+        <v>17891</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>1415</v>
+      </c>
+      <c r="R3" s="5">
+        <v>4862</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="8">
+        <v>44697.391111111108</v>
+      </c>
+      <c r="V3" s="6">
+        <v>7706569020802</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>1136</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>20</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>1137</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="5">
+        <v>30020376</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="I4" s="5">
+        <v>6</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K4" s="7">
+        <v>17891</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>1415</v>
+      </c>
+      <c r="R4" s="5">
+        <v>4862</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="8">
+        <v>44697.391111111108</v>
+      </c>
+      <c r="V4" s="6">
+        <v>7702184010969</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>10</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>20</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="BC4" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5">
+        <v>30020376</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>1414</v>
+      </c>
+      <c r="I5" s="5">
+        <v>6</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="7">
+        <v>17891</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>1415</v>
+      </c>
+      <c r="R5" s="5">
+        <v>4862</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" s="8">
+        <v>44697.391111111108</v>
+      </c>
+      <c r="V5" s="6">
+        <v>7707019459036</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="AD5" s="5">
         <v>1</v>
       </c>
-      <c r="AE2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AE5" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AK5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AL5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AO5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3">
-        <v>1029409136</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="1">
-        <v>43754</v>
-      </c>
-      <c r="M3" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3">
-        <v>5507</v>
-      </c>
-      <c r="S3" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="2">
-        <v>44712.42292824074</v>
-      </c>
-      <c r="V3" s="4">
-        <v>7702605184460</v>
-      </c>
-      <c r="W3" t="s">
-        <v>82</v>
-      </c>
-      <c r="X3" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB3">
-        <v>3</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD3">
-        <v>6</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4">
-        <v>1029409136</v>
-      </c>
-      <c r="H4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
-      </c>
-      <c r="J4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" s="1">
-        <v>43754</v>
-      </c>
-      <c r="M4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N4" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4">
-        <v>5507</v>
-      </c>
-      <c r="S4" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" s="2">
-        <v>44712.42292824074</v>
-      </c>
-      <c r="V4" s="4">
-        <v>7707177970695</v>
-      </c>
-      <c r="W4" t="s">
-        <v>91</v>
-      </c>
-      <c r="X4" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB4">
-        <v>30</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD4">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>30019936</v>
-      </c>
-      <c r="H5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" s="1">
-        <v>20040</v>
-      </c>
-      <c r="M5" t="s">
-        <v>63</v>
-      </c>
-      <c r="N5" t="s">
-        <v>64</v>
-      </c>
-      <c r="P5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>103</v>
-      </c>
-      <c r="R5">
-        <v>5496</v>
-      </c>
-      <c r="S5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" s="2">
-        <v>44712.42292824074</v>
-      </c>
-      <c r="V5" s="4">
-        <v>7707019352610</v>
-      </c>
-      <c r="W5" t="s">
-        <v>104</v>
-      </c>
-      <c r="X5" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB5">
-        <v>30</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD5">
-        <v>30</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>112</v>
-      </c>
-      <c r="AH5">
-        <v>0</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>113</v>
-      </c>
-      <c r="BC5" t="s">
+      <c r="AT5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="BC5" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -52539,19 +52541,19 @@
         <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>1411</v>
       </c>
       <c r="D6" t="s">
         <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="G6">
-        <v>30019936</v>
+        <v>1117458585</v>
       </c>
       <c r="H6" t="s">
-        <v>101</v>
+        <v>1255</v>
       </c>
       <c r="I6">
         <v>6</v>
@@ -52560,7 +52562,7 @@
         <v>102</v>
       </c>
       <c r="K6" s="1">
-        <v>20040</v>
+        <v>39106</v>
       </c>
       <c r="M6" t="s">
         <v>63</v>
@@ -52572,52 +52574,52 @@
         <v>65</v>
       </c>
       <c r="Q6" t="s">
-        <v>103</v>
+        <v>1412</v>
       </c>
       <c r="R6">
-        <v>5496</v>
+        <v>4865</v>
       </c>
       <c r="S6" t="s">
         <v>67</v>
       </c>
       <c r="T6" s="2">
-        <v>44712.42292824074</v>
+        <v>44697.402997685182</v>
       </c>
       <c r="V6" s="4">
-        <v>7702605184453</v>
+        <v>7707177972125</v>
       </c>
       <c r="W6" t="s">
-        <v>114</v>
+        <v>790</v>
       </c>
       <c r="X6" t="s">
-        <v>115</v>
+        <v>791</v>
       </c>
       <c r="Y6" t="s">
-        <v>116</v>
+        <v>239</v>
       </c>
       <c r="Z6" t="s">
         <v>85</v>
       </c>
       <c r="AA6" t="s">
-        <v>117</v>
+        <v>240</v>
       </c>
       <c r="AB6">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="AC6" t="s">
-        <v>109</v>
+        <v>262</v>
       </c>
       <c r="AD6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AE6" t="s">
-        <v>118</v>
+        <v>242</v>
       </c>
       <c r="AF6" t="s">
-        <v>119</v>
+        <v>243</v>
       </c>
       <c r="AG6" t="s">
-        <v>120</v>
+        <v>244</v>
       </c>
       <c r="AH6">
         <v>0</v>
@@ -52641,241 +52643,9 @@
         <v>0</v>
       </c>
       <c r="BB6" t="s">
-        <v>121</v>
+        <v>793</v>
       </c>
       <c r="BC6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>30019936</v>
-      </c>
-      <c r="H7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>102</v>
-      </c>
-      <c r="K7" s="1">
-        <v>20040</v>
-      </c>
-      <c r="M7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N7" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>103</v>
-      </c>
-      <c r="R7">
-        <v>5496</v>
-      </c>
-      <c r="S7" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" s="2">
-        <v>44712.42292824074</v>
-      </c>
-      <c r="V7" s="4">
-        <v>7707019325423</v>
-      </c>
-      <c r="W7" t="s">
-        <v>122</v>
-      </c>
-      <c r="X7" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>124</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB7">
-        <v>30</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD7">
-        <v>60</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH7">
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>128</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>30019936</v>
-      </c>
-      <c r="H8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>102</v>
-      </c>
-      <c r="K8" s="1">
-        <v>20040</v>
-      </c>
-      <c r="M8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N8" t="s">
-        <v>64</v>
-      </c>
-      <c r="P8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>103</v>
-      </c>
-      <c r="R8">
-        <v>5496</v>
-      </c>
-      <c r="S8" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="2">
-        <v>44712.42292824074</v>
-      </c>
-      <c r="V8" s="4">
-        <v>7702605184736</v>
-      </c>
-      <c r="W8" t="s">
-        <v>129</v>
-      </c>
-      <c r="X8" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB8">
-        <v>30</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD8">
-        <v>30</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>133</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>134</v>
-      </c>
-      <c r="BC8" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>